<commit_message>
design all pages corrections
</commit_message>
<xml_diff>
--- a/url_list.xlsx
+++ b/url_list.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="14">
   <si>
     <t>URL TYPE</t>
   </si>
@@ -34,13 +34,39 @@
   </si>
   <si>
     <t>http://192.168.100.19/thaimaiapp/api/mother/mPrimaryInfo/</t>
+  </si>
+  <si>
+    <t>PARAMETERS</t>
+  </si>
+  <si>
+    <t>URL Name</t>
+  </si>
+  <si>
+    <t>POST</t>
+  </si>
+  <si>
+    <t>GET</t>
+  </si>
+  <si>
+    <t>picme_id,
+dob</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> "status": 0
+"message":""</t>
+  </si>
+  <si>
+    <t>DASHBOARD</t>
+  </si>
+  <si>
+    <t>http://192.168.100.19/thaimaiapp/api/mother/mDashboard</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -54,6 +80,21 @@
       <color theme="1"/>
       <name val="Times New Roman"/>
       <family val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -73,14 +114,32 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top"/>
+      <protection locked="0"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -373,45 +432,80 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="26.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="57" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="22.5703125" customWidth="1"/>
+    <col min="2" max="2" width="26.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="57" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="32.7109375" customWidth="1"/>
+    <col min="5" max="5" width="18.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:5">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
+      <c r="D1" s="2" t="s">
+        <v>6</v>
+      </c>
     </row>
-    <row r="2" spans="1:2">
-      <c r="A2" t="s">
+    <row r="2" spans="1:5" ht="58.5" customHeight="1">
+      <c r="A2" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" s="4" t="s">
         <v>3</v>
       </c>
+      <c r="D2" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>11</v>
+      </c>
     </row>
-    <row r="3" spans="1:2">
-      <c r="A3" t="s">
+    <row r="3" spans="1:5" ht="58.5" customHeight="1">
+      <c r="A3" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" s="6" t="s">
         <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>13</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C3" r:id="rId1"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
changes in design all pages and Near By Hospital
</commit_message>
<xml_diff>
--- a/url_list.xlsx
+++ b/url_list.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="16">
   <si>
     <t>URL TYPE</t>
   </si>
@@ -60,6 +60,12 @@
   </si>
   <si>
     <t>http://192.168.100.19/thaimaiapp/api/mother/mDashboard</t>
+  </si>
+  <si>
+    <t>http://192.168.100.19/thaimaiapp/api/mother/mPrimaryInfoUpdate</t>
+  </si>
+  <si>
+    <t>PRIMARY REGISTRATION Update</t>
   </si>
 </sst>
 </file>
@@ -432,17 +438,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="22.5703125" customWidth="1"/>
-    <col min="2" max="2" width="26.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="57" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="29.140625" customWidth="1"/>
+    <col min="3" max="3" width="62.85546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="32.7109375" customWidth="1"/>
     <col min="5" max="5" width="18.7109375" customWidth="1"/>
   </cols>
@@ -498,6 +504,17 @@
       </c>
       <c r="C4" s="3" t="s">
         <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="36.75" customHeight="1">
+      <c r="A5" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Delivery entry api call
</commit_message>
<xml_diff>
--- a/url_list.xlsx
+++ b/url_list.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="23">
   <si>
     <t>URL TYPE</t>
   </si>
@@ -76,13 +76,25 @@
   <si>
     <t>picmeId=1000000000001
 mid=1</t>
+  </si>
+  <si>
+    <t>http://192.168.100.19/thaimaiapp/api/mother/mPN_Record</t>
+  </si>
+  <si>
+    <t>PN Records</t>
+  </si>
+  <si>
+    <t>http://192.168.100.19/thaimaiapp/api/mother/mDeleveryDetailsInsert</t>
+  </si>
+  <si>
+    <t>Delivery Insert</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -112,6 +124,12 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -137,7 +155,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -151,6 +169,9 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -448,17 +469,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E6"/>
+  <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="22.5703125" customWidth="1"/>
     <col min="2" max="2" width="29.140625" customWidth="1"/>
-    <col min="3" max="3" width="62.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="66.85546875" customWidth="1"/>
     <col min="4" max="4" width="32.7109375" customWidth="1"/>
     <col min="5" max="5" width="18.7109375" customWidth="1"/>
   </cols>
@@ -535,6 +556,31 @@
         <v>16</v>
       </c>
       <c r="D6" s="5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="30">
+      <c r="B7" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="30">
+      <c r="A8" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="C8" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="D8" s="5" t="s">
         <v>18</v>
       </c>
     </row>

</xml_diff>

<commit_message>
delivery Entry Changes, PNHBNC VISIT Changes, API CALL
</commit_message>
<xml_diff>
--- a/url_list.xlsx
+++ b/url_list.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="31">
   <si>
     <t>URL TYPE</t>
   </si>
@@ -27,13 +27,7 @@
     <t>LOGIN</t>
   </si>
   <si>
-    <t>http://192.168.100.19/thaimaiapp/api/login/check/</t>
-  </si>
-  <si>
     <t>PRIMARY REGISTRATION URL</t>
-  </si>
-  <si>
-    <t>http://192.168.100.19/thaimaiapp/api/mother/mPrimaryInfo/</t>
   </si>
   <si>
     <t>PARAMETERS</t>
@@ -59,16 +53,7 @@
     <t>DASHBOARD</t>
   </si>
   <si>
-    <t>http://192.168.100.19/thaimaiapp/api/mother/mDashboard</t>
-  </si>
-  <si>
-    <t>http://192.168.100.19/thaimaiapp/api/mother/mPrimaryInfoUpdate</t>
-  </si>
-  <si>
     <t>PRIMARY REGISTRATION Update</t>
-  </si>
-  <si>
-    <t>http://192.168.100.19/thaimaiapp/api/mother/mHealthRecord</t>
   </si>
   <si>
     <t>HEALTH RECORDS</t>
@@ -78,23 +63,62 @@
 mid=1</t>
   </si>
   <si>
-    <t>http://192.168.100.19/thaimaiapp/api/mother/mPN_Record</t>
-  </si>
-  <si>
     <t>PN Records</t>
   </si>
   <si>
-    <t>http://192.168.100.19/thaimaiapp/api/mother/mDeleveryDetailsInsert</t>
-  </si>
-  <si>
     <t>Delivery Insert</t>
+  </si>
+  <si>
+    <t>Delivery Details</t>
+  </si>
+  <si>
+    <t>LOCATION Update</t>
+  </si>
+  <si>
+    <t>PN Helath Records</t>
+  </si>
+  <si>
+    <t>Visit Number</t>
+  </si>
+  <si>
+    <t>http://192.168.100.235/thaimaiapp/api/mother/mPrimaryInfo/</t>
+  </si>
+  <si>
+    <t>http://192.168.100.235/thaimaiapp/api/mother/mDashboard</t>
+  </si>
+  <si>
+    <t>http://192.168.100.235/thaimaiapp/api/mother/mPrimaryInfoUpdate</t>
+  </si>
+  <si>
+    <t>http://192.168.100.235/thaimaiapp/api/mother/mHealthRecord</t>
+  </si>
+  <si>
+    <t>http://192.168.100.235/thaimaiapp/api/mother/mPN_Record</t>
+  </si>
+  <si>
+    <t>http://192.168.100.235/thaimaiapp/api/mother/mDeleveryDetailsInsert</t>
+  </si>
+  <si>
+    <t>http://192.168.100.235/thaimaiapp/api/mother/mDeleveryDetails</t>
+  </si>
+  <si>
+    <t>http://192.168.100.235/thaimaiapp/api/mother/mPN_Record_Insert</t>
+  </si>
+  <si>
+    <t>http://192.168.100.235/thaimaiapp/api/mother/locationUpdate</t>
+  </si>
+  <si>
+    <t>http://192.168.100.235/thaimaiapp/api/mother/mHealthRecordVisitNumber</t>
+  </si>
+  <si>
+    <t>http://192.168.100.235/thaimaiapp/api/login/check/</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="5">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -124,12 +148,6 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -155,7 +173,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -171,9 +189,10 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -469,10 +488,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E8"/>
+  <dimension ref="A1:E12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -489,107 +508,151 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="58.5" customHeight="1">
       <c r="A2" s="4" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="4" t="s">
-        <v>3</v>
+      <c r="C2" s="6" t="s">
+        <v>30</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="58.5" customHeight="1">
       <c r="A3" s="4" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>5</v>
+        <v>20</v>
       </c>
     </row>
     <row r="4" spans="1:5">
       <c r="A4" s="3" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>13</v>
+        <v>21</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="36.75" customHeight="1">
       <c r="A5" s="4" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="30">
       <c r="B6" s="4" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="30">
       <c r="B7" s="4" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="C7" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="30">
+      <c r="A8" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C8" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="35.25" customHeight="1">
+      <c r="A9" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C9" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="26.25" customHeight="1">
+      <c r="B10" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C10" s="7" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="28.5" customHeight="1">
+      <c r="B11" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C11" s="7" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="28.5" customHeight="1">
+      <c r="B12" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="D7" s="5" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" ht="30">
-      <c r="A8" t="s">
-        <v>8</v>
-      </c>
-      <c r="B8" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="C8" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="D8" s="5" t="s">
-        <v>18</v>
+      <c r="C12" s="8" t="s">
+        <v>29</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C3" r:id="rId1"/>
+    <hyperlink ref="C3" r:id="rId1" display="http://192.168.100.19/thaimaiapp/api/mother/mPrimaryInfo/"/>
+    <hyperlink ref="C8" r:id="rId2" display="http://192.168.100.19/thaimaiapp/api/mother/mDeleveryDetailsInsert"/>
+    <hyperlink ref="C10" r:id="rId3" display="http://192.168.100.19/thaimaiapp/api/mother/mPN_Record_Insert"/>
+    <hyperlink ref="C11" r:id="rId4" display="http://192.168.100.19/thaimaiapp/api/mother/locationUpdate"/>
+    <hyperlink ref="C9" r:id="rId5" display="http://192.168.100.19/thaimaiapp/api/mother/mDeleveryDetails"/>
+    <hyperlink ref="C12" r:id="rId6" display="http://192.168.100.19/thaimaiapp/api/mother/mHealthRecordVisitNumber"/>
+    <hyperlink ref="C2" r:id="rId7" display="http://192.168.100.19/thaimaiapp/api/login/check/"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId2"/>
+  <pageSetup orientation="portrait" r:id="rId8"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Pn-hbnc screen api call and UI Changes.
</commit_message>
<xml_diff>
--- a/url_list.xlsx
+++ b/url_list.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="26">
   <si>
     <t>URL TYPE</t>
   </si>
@@ -88,6 +88,17 @@
   </si>
   <si>
     <t>Delivery Insert</t>
+  </si>
+  <si>
+    <t>http://192.168.100.19/thaimaiapp/api/mother/locationUpdate</t>
+  </si>
+  <si>
+    <t>mPicmeId:1000000000001
+latitude:12
+longitude:11</t>
+  </si>
+  <si>
+    <t>Location Update</t>
   </si>
 </sst>
 </file>
@@ -131,12 +142,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -155,7 +172,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -172,6 +189,12 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -469,10 +492,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E8"/>
+  <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -582,6 +605,17 @@
       </c>
       <c r="D8" s="5" t="s">
         <v>18</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="45">
+      <c r="B9" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C9" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="D9" s="8" t="s">
+        <v>24</v>
       </c>
     </row>
   </sheetData>

</xml_diff>